<commit_message>
Added to the manuscript
</commit_message>
<xml_diff>
--- a/data/utils/summary_column_names.xlsx
+++ b/data/utils/summary_column_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhgille2\Documents\R\projects\Jay_yield\data\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\R\Projects\Jay_yield\data\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C5DA80-6D45-44C7-8F54-726317A75895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E270BE9C-F5A2-4A5D-9E5A-CFE0AECD9A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53070" yWindow="2295" windowWidth="21600" windowHeight="11325" xr2:uid="{A039830A-5F9D-4F95-B54A-099372331C43}"/>
+    <workbookView xWindow="9600" yWindow="5500" windowWidth="28800" windowHeight="15500" xr2:uid="{A039830A-5F9D-4F95-B54A-099372331C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>old_name</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>HSD</t>
+  </si>
+  <si>
+    <t>test_name</t>
+  </si>
+  <si>
+    <t>Test Name</t>
   </si>
 </sst>
 </file>
@@ -428,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8CA5E2-478C-4AD1-AC9E-7C2B521711F4}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -452,7 +458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -460,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -468,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -476,7 +482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -484,12 +490,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>